<commit_message>
Changed the Test Status
</commit_message>
<xml_diff>
--- a/HybridRediff/Files/StockSuite.xlsx
+++ b/HybridRediff/Files/StockSuite.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01919272-679B-429A-A78E-5AE2FCF16BC6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="40">
   <si>
     <t>TCID</t>
   </si>
@@ -133,13 +134,16 @@
   </si>
   <si>
     <t>Tata Steel Ltd</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +247,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -289,7 +301,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -321,9 +333,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -355,6 +385,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -530,19 +578,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -550,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -558,7 +606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -566,20 +614,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -589,24 +637,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -626,7 +674,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -640,7 +688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -654,7 +702,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -666,7 +714,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -682,7 +730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -694,7 +742,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -706,7 +754,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
@@ -720,7 +768,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
@@ -734,7 +782,7 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>4</v>
       </c>
@@ -746,7 +794,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
@@ -762,7 +810,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>4</v>
       </c>
@@ -774,7 +822,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>4</v>
       </c>
@@ -786,7 +834,7 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
@@ -800,7 +848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -814,7 +862,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -826,7 +874,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -842,7 +890,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -854,7 +902,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -866,7 +914,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>35</v>
       </c>
@@ -880,7 +928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>35</v>
       </c>
@@ -894,7 +942,7 @@
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>35</v>
       </c>
@@ -906,7 +954,7 @@
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>35</v>
       </c>
@@ -922,7 +970,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>35</v>
       </c>
@@ -934,7 +982,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>35</v>
       </c>
@@ -953,31 +1001,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1000,7 +1048,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1023,12 +1071,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
@@ -1042,7 +1090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1056,12 +1104,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
@@ -1087,7 +1135,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1113,12 +1161,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>1</v>
       </c>
@@ -1132,7 +1180,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>

</xml_diff>